<commit_message>
New full screen layout
</commit_message>
<xml_diff>
--- a/01_Beschrijvingen.xlsx
+++ b/01_Beschrijvingen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Spanish</t>
   </si>
@@ -22,136 +22,202 @@
     <t>English</t>
   </si>
   <si>
+    <t>Tonto</t>
+  </si>
+  <si>
+    <t>Tímido</t>
+  </si>
+  <si>
+    <t>Insensible</t>
+  </si>
+  <si>
+    <t>Borde</t>
+  </si>
+  <si>
+    <t>Perezoso</t>
+  </si>
+  <si>
     <t>Tacaño</t>
   </si>
   <si>
-    <t>Limpio</t>
+    <t>Triste</t>
+  </si>
+  <si>
+    <t>Incómodo</t>
+  </si>
+  <si>
+    <t>Grosero</t>
+  </si>
+  <si>
+    <t>Aburrido</t>
+  </si>
+  <si>
+    <t>Ancho</t>
   </si>
   <si>
     <t>Valiente</t>
   </si>
   <si>
+    <t>Mayor</t>
+  </si>
+  <si>
+    <t>Delgado</t>
+  </si>
+  <si>
+    <t>Callado</t>
+  </si>
+  <si>
+    <t>Simpático</t>
+  </si>
+  <si>
+    <t>Mentiroso</t>
+  </si>
+  <si>
+    <t>Ligero</t>
+  </si>
+  <si>
+    <t>Desagradable</t>
+  </si>
+  <si>
+    <t>Antipático</t>
+  </si>
+  <si>
+    <t>Oscuro</t>
+  </si>
+  <si>
+    <t>Pesado</t>
+  </si>
+  <si>
+    <t>Ruidoso</t>
+  </si>
+  <si>
+    <t>Amable</t>
+  </si>
+  <si>
+    <t>Bajo</t>
+  </si>
+  <si>
+    <t>Rubio</t>
+  </si>
+  <si>
+    <t>Vago</t>
+  </si>
+  <si>
+    <t>Alegre</t>
+  </si>
+  <si>
     <t>Estrecho</t>
   </si>
   <si>
+    <t>Extravertido</t>
+  </si>
+  <si>
     <t>Cobarde</t>
   </si>
   <si>
     <t>Sensible</t>
   </si>
   <si>
-    <t>Creído</t>
-  </si>
-  <si>
-    <t>Cómodo</t>
-  </si>
-  <si>
-    <t>Perezoso</t>
-  </si>
-  <si>
-    <t>Callado</t>
-  </si>
-  <si>
-    <t>Incómodo</t>
-  </si>
-  <si>
-    <t>Grosero</t>
-  </si>
-  <si>
-    <t>Mentiroso</t>
-  </si>
-  <si>
-    <t>Delgado</t>
-  </si>
-  <si>
-    <t>Pesado</t>
-  </si>
-  <si>
-    <t>Desagradable</t>
-  </si>
-  <si>
-    <t>Oscuro</t>
-  </si>
-  <si>
-    <t>Agradable</t>
-  </si>
-  <si>
-    <t>Vago</t>
-  </si>
-  <si>
-    <t>Aburrido</t>
-  </si>
-  <si>
-    <t>Ruidoso</t>
-  </si>
-  <si>
-    <t>Modesto</t>
+    <t>Ordenado</t>
+  </si>
+  <si>
+    <t>silly/foolish/dumb</t>
+  </si>
+  <si>
+    <t>shy</t>
+  </si>
+  <si>
+    <t>insensitive</t>
+  </si>
+  <si>
+    <t>rude (colloquial)</t>
+  </si>
+  <si>
+    <t>lazy</t>
   </si>
   <si>
     <t>stingy</t>
   </si>
   <si>
-    <t>clean</t>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>uncomfortable</t>
+  </si>
+  <si>
+    <t>rude</t>
+  </si>
+  <si>
+    <t>boring</t>
+  </si>
+  <si>
+    <t>wide</t>
   </si>
   <si>
     <t>brave</t>
   </si>
   <si>
+    <t>older (age)</t>
+  </si>
+  <si>
+    <t>thin/slim</t>
+  </si>
+  <si>
+    <t>quiet</t>
+  </si>
+  <si>
+    <t>nice/friendly</t>
+  </si>
+  <si>
+    <t>lying/dishonest</t>
+  </si>
+  <si>
+    <t>light (weight)</t>
+  </si>
+  <si>
+    <t>unpleasant</t>
+  </si>
+  <si>
+    <t>unfriendly/unpleasant</t>
+  </si>
+  <si>
+    <t>dark</t>
+  </si>
+  <si>
+    <t>heavy</t>
+  </si>
+  <si>
+    <t>noisy/loud</t>
+  </si>
+  <si>
+    <t>kind/friendly</t>
+  </si>
+  <si>
+    <t>short (in height)</t>
+  </si>
+  <si>
+    <t>blond(e)</t>
+  </si>
+  <si>
+    <t>lazy (colloquial)</t>
+  </si>
+  <si>
+    <t>cheerful/happy</t>
+  </si>
+  <si>
     <t>narrow</t>
   </si>
   <si>
+    <t>extroverted/outgoing</t>
+  </si>
+  <si>
     <t>cowardly/coward</t>
   </si>
   <si>
     <t>sensitive</t>
   </si>
   <si>
-    <t>conceited</t>
-  </si>
-  <si>
-    <t>comfortable</t>
-  </si>
-  <si>
-    <t>lazy</t>
-  </si>
-  <si>
-    <t>quiet</t>
-  </si>
-  <si>
-    <t>uncomfortable</t>
-  </si>
-  <si>
-    <t>rude</t>
-  </si>
-  <si>
-    <t>lying/dishonest</t>
-  </si>
-  <si>
-    <t>thin/slim</t>
-  </si>
-  <si>
-    <t>heavy</t>
-  </si>
-  <si>
-    <t>unpleasant</t>
-  </si>
-  <si>
-    <t>dark</t>
-  </si>
-  <si>
-    <t>pleasant</t>
-  </si>
-  <si>
-    <t>lazy (colloquial)</t>
-  </si>
-  <si>
-    <t>boring</t>
-  </si>
-  <si>
-    <t>noisy/loud</t>
-  </si>
-  <si>
-    <t>modest</t>
+    <t>tidy/organized</t>
   </si>
 </sst>
 </file>
@@ -509,7 +575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -528,7 +594,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -536,7 +602,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -544,7 +610,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -552,7 +618,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -560,7 +626,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -568,7 +634,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -576,7 +642,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -584,7 +650,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -592,7 +658,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -600,7 +666,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -608,7 +674,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -616,7 +682,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -624,7 +690,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -632,7 +698,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -640,7 +706,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -648,7 +714,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -656,7 +722,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -664,7 +730,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -672,7 +738,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -680,7 +746,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -688,7 +754,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -696,7 +762,95 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>